<commit_message>
Reworked the proposed solution
</commit_message>
<xml_diff>
--- a/NewProjects/GrossProfit/Costing.xlsx
+++ b/NewProjects/GrossProfit/Costing.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Cloud\OneDrive\Eniac\Engineparts\NewProjects\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Users\GitHub\ep\NewProjects\GrossProfit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F37AE713-5DE7-4738-A497-419475EDC76E}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A68C7B65-2F9F-4B1D-8428-3C4B709E4A8D}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12750" xr2:uid="{92D01F5E-3596-4C9D-9917-CF1D18247172}"/>
   </bookViews>
@@ -23,6 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -107,7 +108,7 @@
     <t>Setup &amp; Implementation</t>
   </si>
   <si>
-    <t>Invetment estimate</t>
+    <t>Investment estimate</t>
   </si>
 </sst>
 </file>
@@ -116,7 +117,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -162,7 +163,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -205,37 +206,61 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -246,7 +271,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -258,6 +283,13 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -581,16 +613,16 @@
   <dimension ref="C1:N29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="4.5703125" style="19" customWidth="1"/>
+    <col min="3" max="3" width="4.5703125" style="17" customWidth="1"/>
     <col min="4" max="4" width="39.42578125" customWidth="1"/>
     <col min="5" max="5" width="9.140625" customWidth="1"/>
     <col min="6" max="6" width="13.42578125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="3.7109375" style="19" customWidth="1"/>
+    <col min="10" max="10" width="3.7109375" style="17" customWidth="1"/>
     <col min="11" max="11" width="37.42578125" customWidth="1"/>
     <col min="14" max="14" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
   </cols>
@@ -601,7 +633,7 @@
       <c r="N1" s="7"/>
     </row>
     <row r="2" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C2" s="17" t="s">
+      <c r="C2" s="15" t="s">
         <v>10</v>
       </c>
       <c r="D2" s="12" t="s">
@@ -613,7 +645,7 @@
       <c r="F2" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="J2" s="17" t="s">
+      <c r="J2" s="15" t="s">
         <v>10</v>
       </c>
       <c r="K2" s="12" t="s">
@@ -630,7 +662,7 @@
       </c>
     </row>
     <row r="3" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C3" s="18">
+      <c r="C3" s="16">
         <v>1</v>
       </c>
       <c r="D3" s="8" t="s">
@@ -640,7 +672,7 @@
       <c r="F3" s="9">
         <v>22000000</v>
       </c>
-      <c r="J3" s="18">
+      <c r="J3" s="16">
         <v>1</v>
       </c>
       <c r="K3" s="8" t="s">
@@ -658,7 +690,7 @@
       </c>
     </row>
     <row r="4" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C4" s="18">
+      <c r="C4" s="16">
         <v>2</v>
       </c>
       <c r="D4" s="8" t="s">
@@ -671,7 +703,7 @@
         <f>F3*E4</f>
         <v>5940000</v>
       </c>
-      <c r="J4" s="18">
+      <c r="J4" s="16">
         <v>2</v>
       </c>
       <c r="K4" s="8" t="s">
@@ -689,7 +721,7 @@
       </c>
     </row>
     <row r="5" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C5" s="18">
+      <c r="C5" s="16">
         <v>3</v>
       </c>
       <c r="D5" s="8" t="s">
@@ -702,7 +734,7 @@
         <f>F3*E5</f>
         <v>6269999.9999999991</v>
       </c>
-      <c r="J5" s="18">
+      <c r="J5" s="16">
         <v>3</v>
       </c>
       <c r="K5" s="8" t="s">
@@ -719,19 +751,17 @@
         <v>36000</v>
       </c>
     </row>
-    <row r="6" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C6" s="18">
-        <v>4</v>
-      </c>
-      <c r="D6" s="15" t="s">
+    <row r="6" spans="3:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C6" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="E6" s="15"/>
-      <c r="F6" s="16">
+      <c r="D6" s="25"/>
+      <c r="E6" s="26"/>
+      <c r="F6" s="27">
         <f>F5-F4</f>
         <v>329999.99999999907</v>
       </c>
-      <c r="J6" s="18">
+      <c r="J6" s="16">
         <v>4</v>
       </c>
       <c r="K6" s="8" t="s">
@@ -748,8 +778,8 @@
         <v>7200</v>
       </c>
     </row>
-    <row r="7" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="J7" s="18">
+    <row r="7" spans="3:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="J7" s="16">
         <v>5</v>
       </c>
       <c r="K7" s="8" t="s">
@@ -767,7 +797,7 @@
       </c>
     </row>
     <row r="8" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="J8" s="18">
+      <c r="J8" s="16">
         <v>6</v>
       </c>
       <c r="K8" s="8" t="s">
@@ -785,30 +815,30 @@
       </c>
     </row>
     <row r="9" spans="3:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J9" s="25"/>
-      <c r="K9" s="26" t="s">
+      <c r="J9" s="23"/>
+      <c r="K9" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="L9" s="26"/>
-      <c r="M9" s="26"/>
-      <c r="N9" s="21">
+      <c r="L9" s="24"/>
+      <c r="M9" s="24"/>
+      <c r="N9" s="19">
         <f>SUM(N3:N8)</f>
         <v>108000</v>
       </c>
     </row>
     <row r="10" spans="3:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="J10" s="25"/>
-      <c r="K10" s="23"/>
-      <c r="L10" s="23"/>
-      <c r="M10" s="23"/>
+      <c r="J10" s="23"/>
+      <c r="K10" s="21"/>
+      <c r="L10" s="21"/>
+      <c r="M10" s="21"/>
     </row>
     <row r="11" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="J11" s="22"/>
-      <c r="K11" s="23"/>
+      <c r="J11" s="20"/>
+      <c r="K11" s="21"/>
     </row>
     <row r="12" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="J12" s="22"/>
-      <c r="K12" s="23"/>
+      <c r="J12" s="20"/>
+      <c r="K12" s="21"/>
     </row>
     <row r="13" spans="3:14" x14ac:dyDescent="0.25">
       <c r="D13" t="s">
@@ -817,8 +847,8 @@
       <c r="F13" s="1">
         <v>20000000</v>
       </c>
-      <c r="J13" s="22"/>
-      <c r="K13" s="24"/>
+      <c r="J13" s="20"/>
+      <c r="K13" s="22"/>
     </row>
     <row r="14" spans="3:14" x14ac:dyDescent="0.25">
       <c r="D14" t="s">
@@ -831,8 +861,8 @@
         <f>F13*E14</f>
         <v>6400000</v>
       </c>
-      <c r="J14" s="22"/>
-      <c r="K14" s="24"/>
+      <c r="J14" s="20"/>
+      <c r="K14" s="22"/>
     </row>
     <row r="15" spans="3:14" x14ac:dyDescent="0.25">
       <c r="D15" t="s">
@@ -843,7 +873,7 @@
         <f>F5</f>
         <v>6269999.9999999991</v>
       </c>
-      <c r="K15" s="20"/>
+      <c r="K15" s="18"/>
     </row>
     <row r="16" spans="3:14" x14ac:dyDescent="0.25">
       <c r="D16" t="s">
@@ -959,8 +989,9 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="K9:M9"/>
+    <mergeCell ref="C6:E6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>